<commit_message>
php: create empty file and with demo data
</commit_message>
<xml_diff>
--- a/web/documentserver-example/php/app_data/demo.xlsx
+++ b/web/documentserver-example/php/app_data/demo.xlsx
@@ -36,76 +36,76 @@
     <t>USA</t>
   </si>
   <si>
+    <t>China</t>
+  </si>
+  <si>
     <t xml:space="preserve">Great Britain</t>
   </si>
   <si>
-    <t>China</t>
-  </si>
-  <si>
     <t>Russia</t>
   </si>
   <si>
+    <t xml:space="preserve">South Korea</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Korea</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>Australia</t>
+    <t>Kazakhstan</t>
   </si>
   <si>
     <t>Netherlands</t>
   </si>
   <si>
-    <t>Hungary</t>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Zealand</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czech Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Korea</t>
+  </si>
+  <si>
+    <t>Spain</t>
   </si>
   <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Jamaica</t>
+    <t xml:space="preserve">South Africa</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
   </si>
   <si>
     <t>Croatia</t>
-  </si>
-  <si>
-    <t>Cuba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Zealand</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>Uzbekistan</t>
-  </si>
-  <si>
-    <t>Kazakhstan</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Iran</t>
   </si>
   <si>
     <t>Total:</t>
@@ -117,62 +117,62 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
-      <color theme="1"/>
+      <scheme val="none"/>
       <sz val="8"/>
-      <scheme val="none"/>
     </font>
     <font>
+      <color theme="0"/>
       <name val="Arial"/>
-      <color theme="0"/>
+      <scheme val="minor"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
-      <color theme="1"/>
+      <scheme val="none"/>
       <sz val="12"/>
-      <scheme val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
       <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="none"/>
       <sz val="12"/>
-      <scheme val="none"/>
     </font>
     <font>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color indexed="64"/>
+      <scheme val="none"/>
       <sz val="13"/>
-      <scheme val="none"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b/>
       <color indexed="64"/>
+      <name val="Calibri"/>
+      <scheme val="none"/>
       <sz val="13"/>
-      <scheme val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
       <b/>
       <color indexed="64"/>
+      <name val="Arial"/>
+      <scheme val="none"/>
       <sz val="12"/>
-      <scheme val="none"/>
     </font>
     <font>
+      <color rgb="FF434343"/>
       <name val="Arial"/>
-      <color rgb="FF434343"/>
+      <scheme val="none"/>
       <sz val="12"/>
-      <scheme val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
       <b/>
       <color rgb="FF434343"/>
+      <name val="Arial"/>
+      <scheme val="none"/>
       <sz val="12"/>
-      <scheme val="none"/>
     </font>
   </fonts>
   <fills count="9">
@@ -208,8 +208,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.049989318521683403"/>
-        <bgColor theme="0" tint="-0.049989318521683403"/>
+        <fgColor theme="0" tint="-4.9989318521683403e-002"/>
+        <bgColor theme="0" tint="-4.9989318521683403e-002"/>
       </patternFill>
     </fill>
     <fill>
@@ -476,11 +476,11 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -513,8 +513,8 @@
     <c:plotArea>
       <c:layout/>
       <c:areaChart>
+        <c:varyColors val="0"/>
         <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -537,14 +537,7 @@
               <a:srgbClr val="2DA2BF"/>
             </a:solidFill>
           </c:spPr>
-          <c:dLbls>
-            <c:showBubbleSize val="0"/>
-            <c:showCatName val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!C3:C27</c:f>
@@ -554,80 +547,88 @@
                   <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v xml:space="preserve">Great Britain</c:v>
+                  <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>China</c:v>
+                  <c:v>Great Britain</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Russia</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Japan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v xml:space="preserve">South Korea</c:v>
+                  <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Italy</c:v>
+                  <c:v>Hungary</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Australia</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Kazakhstan</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Netherlands</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Hungary</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>Ukraine</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>New Zealand</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Cuba</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Jamaica</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Czech Republic</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>North Korea</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Brazil</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>Spain</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Kenya</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Jamaica</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
+                  <c:v>South Africa</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ethiopia</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Croatia</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Cuba</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v xml:space="preserve">New Zealand</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Canada</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Uzbekistan</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Kazakhstan</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Colombia</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Switzerland</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Iran</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!D3:D27</c:f>
@@ -637,55 +638,55 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>4</c:v>
@@ -694,7 +695,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>3</c:v>
@@ -734,14 +735,7 @@
               <a:srgbClr val="DA1F28"/>
             </a:solidFill>
           </c:spPr>
-          <c:dLbls>
-            <c:showBubbleSize val="0"/>
-            <c:showCatName val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!C3:C27</c:f>
@@ -751,147 +745,155 @@
                   <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v xml:space="preserve">Great Britain</c:v>
+                  <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>China</c:v>
+                  <c:v>Great Britain</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Russia</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Japan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v xml:space="preserve">South Korea</c:v>
+                  <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Italy</c:v>
+                  <c:v>Hungary</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Australia</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Kazakhstan</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Netherlands</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Hungary</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>Ukraine</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>New Zealand</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Cuba</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Jamaica</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Czech Republic</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>North Korea</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Brazil</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>Spain</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Kenya</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Jamaica</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
+                  <c:v>South Africa</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ethiopia</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Croatia</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Cuba</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v xml:space="preserve">New Zealand</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Canada</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Uzbekistan</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Kazakhstan</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Colombia</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Switzerland</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Iran</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!E3:E27</c:f>
               <c:numCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>5</c:v>
@@ -900,7 +902,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>1</c:v>
@@ -931,14 +933,7 @@
               <a:srgbClr val="EB641B"/>
             </a:solidFill>
           </c:spPr>
-          <c:dLbls>
-            <c:showBubbleSize val="0"/>
-            <c:showCatName val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!C3:C27</c:f>
@@ -948,171 +943,179 @@
                   <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v xml:space="preserve">Great Britain</c:v>
+                  <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>China</c:v>
+                  <c:v>Great Britain</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Russia</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Japan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v xml:space="preserve">South Korea</c:v>
+                  <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Italy</c:v>
+                  <c:v>Hungary</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Australia</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Kazakhstan</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Netherlands</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>Hungary</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
+                  <c:v>Ukraine</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>New Zealand</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Cuba</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Jamaica</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Czech Republic</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>North Korea</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>Brazil</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>Spain</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Kenya</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Jamaica</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
+                  <c:v>South Africa</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Ethiopia</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>Croatia</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Cuba</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v xml:space="preserve">New Zealand</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Canada</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Uzbekistan</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Kazakhstan</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Colombia</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Switzerland</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Iran</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!F3:F27</c:f>
               <c:numCache>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
         </c:dLbls>
         <c:axId val="7622"/>
         <c:axId val="5026"/>
@@ -1123,10 +1126,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr bwMode="auto"/>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1147,13 +1147,14 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="5026"/>
         <c:crossesAt val="0"/>
+        <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
@@ -1162,10 +1163,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr bwMode="auto"/>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1188,12 +1186,12 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:axPos val="l"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="7622"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1203,24 +1201,15 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-  </c:spPr>
-  <c:externalData r:id="rId1">
-    <c:autoUpdate val="0"/>
-  </c:externalData>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="c14">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -1251,8 +1240,8 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
+        <c:varyColors val="0"/>
         <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1275,17 +1264,7 @@
               <a:srgbClr val="2DA2BF"/>
             </a:solidFill>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showBubbleSize val="0"/>
-            <c:showCatName val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!C3:C12</c:f>
@@ -1295,28 +1274,28 @@
                   <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v xml:space="preserve">Great Britain</c:v>
+                  <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>China</c:v>
+                  <c:v>Great Britain</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Russia</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Japan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v xml:space="preserve">South Korea</c:v>
+                  <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Italy</c:v>
+                  <c:v>Hungary</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Australia</c:v>
@@ -1324,6 +1303,17 @@
               </c:strCache>
             </c:strRef>
           </c:cat>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!D3:D12</c:f>
@@ -1333,31 +1323,31 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1386,17 +1376,7 @@
               <a:srgbClr val="DA1F28"/>
             </a:solidFill>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:showBubbleSize val="0"/>
-            <c:showCatName val="0"/>
-            <c:showLegendKey val="0"/>
-            <c:showPercent val="0"/>
-            <c:showSerName val="0"/>
-            <c:showVal val="0"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!C3:C12</c:f>
@@ -1406,28 +1386,28 @@
                   <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v xml:space="preserve">Great Britain</c:v>
+                  <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>China</c:v>
+                  <c:v>Great Britain</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Russia</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Germany</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Japan</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v xml:space="preserve">South Korea</c:v>
+                  <c:v>Italy</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Italy</c:v>
+                  <c:v>Hungary</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Australia</c:v>
@@ -1435,40 +1415,51 @@
               </c:strCache>
             </c:strRef>
           </c:cat>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!E3:E12</c:f>
               <c:numCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>37</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1477,12 +1468,12 @@
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showCatName val="0"/>
-          <c:showLegendKey val="0"/>
-          <c:showPercent val="0"/>
-          <c:showSerName val="0"/>
-          <c:showVal val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
         <c:axId val="3375"/>
@@ -1494,10 +1485,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr bwMode="auto"/>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1518,13 +1506,14 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="13466"/>
         <c:crossesAt val="0"/>
+        <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
@@ -1533,10 +1522,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr bwMode="auto"/>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1557,12 +1543,12 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:axPos val="l"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="3375"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1572,15 +1558,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
-  <c:spPr bwMode="auto">
-    <a:xfrm>
-      <a:off x="0" y="0"/>
-      <a:ext cx="0" cy="0"/>
-    </a:xfrm>
-  </c:spPr>
-  <c:externalData r:id="rId1">
-    <c:autoUpdate val="0"/>
-  </c:externalData>
 </c:chartSpace>
 </file>
 
@@ -1589,7 +1566,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>9521</xdr:colOff>
+      <xdr:colOff>9522</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1599,12 +1576,10 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>85722</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="1" name="diagram"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1631,12 +1606,10 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>204785</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="1" name="diagram"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1652,32 +1625,30 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>504822</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2238373</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38001</xdr:rowOff>
+      <xdr:rowOff>9520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="0" name=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
-        <a:xfrm flipH="0" flipV="0">
-          <a:off x="1200150" y="0"/>
-          <a:ext cx="2133599" cy="961927"/>
+        <a:xfrm>
+          <a:off x="504822" y="19049"/>
+          <a:ext cx="6619873" cy="914396"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1874,14 +1845,14 @@
         <v>46</v>
       </c>
       <c r="E3" s="14">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F3" s="17">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G3" s="18">
         <f>SUM(D3:F3)</f>
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1899,17 +1870,17 @@
         <v>7</v>
       </c>
       <c r="D4" s="21">
+        <v>38</v>
+      </c>
+      <c r="E4" s="22">
         <v>27</v>
       </c>
-      <c r="E4" s="22">
+      <c r="F4" s="23">
         <v>23</v>
-      </c>
-      <c r="F4" s="23">
-        <v>17</v>
       </c>
       <c r="G4" s="24">
         <f>SUM(D4:F4)</f>
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1927,17 +1898,17 @@
         <v>8</v>
       </c>
       <c r="D5" s="21">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E5" s="22">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="23">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G5" s="24">
         <f>SUM(D5:F5)</f>
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1951,17 +1922,17 @@
         <v>9</v>
       </c>
       <c r="D6" s="21">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E6" s="22">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F6" s="23">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G6" s="24">
         <f>SUM(D6:F6)</f>
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1975,17 +1946,17 @@
         <v>10</v>
       </c>
       <c r="D7" s="21">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" s="22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="23">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G7" s="24">
         <f>SUM(D7:F7)</f>
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2003,17 +1974,17 @@
         <v>11</v>
       </c>
       <c r="D8" s="21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="22">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F8" s="23">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G8" s="24">
         <f>SUM(D8:F8)</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2031,17 +2002,17 @@
         <v>12</v>
       </c>
       <c r="D9" s="21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="22">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F9" s="23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G9" s="24">
         <f>SUM(D9:F9)</f>
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2059,17 +2030,17 @@
         <v>13</v>
       </c>
       <c r="D10" s="21">
+        <v>8</v>
+      </c>
+      <c r="E10" s="22">
         <v>9</v>
       </c>
-      <c r="E10" s="22">
-        <v>3</v>
-      </c>
       <c r="F10" s="23">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G10" s="24">
         <f>SUM(D10:F10)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -2090,14 +2061,14 @@
         <v>8</v>
       </c>
       <c r="E11" s="22">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F11" s="23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G11" s="24">
         <f>SUM(D11:F11)</f>
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -2115,17 +2086,17 @@
         <v>15</v>
       </c>
       <c r="D12" s="21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="22">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F12" s="23">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G12" s="24">
         <f>SUM(D12:F12)</f>
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -2143,17 +2114,17 @@
         <v>16</v>
       </c>
       <c r="D13" s="21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="22">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F13" s="23">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G13" s="24">
         <f>SUM(D13:F13)</f>
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2171,17 +2142,17 @@
         <v>17</v>
       </c>
       <c r="D14" s="21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="24">
         <f>SUM(D14:F14)</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2199,17 +2170,17 @@
         <v>18</v>
       </c>
       <c r="D15" s="21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="22">
         <v>6</v>
       </c>
       <c r="F15" s="23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G15" s="24">
         <f>SUM(D15:F15)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2227,17 +2198,17 @@
         <v>19</v>
       </c>
       <c r="D16" s="21">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F16" s="23">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G16" s="24">
         <f>SUM(D16:F16)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2258,10 +2229,10 @@
         <v>6</v>
       </c>
       <c r="E17" s="22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F17" s="23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G17" s="24">
         <f>SUM(D17:F17)</f>
@@ -2283,17 +2254,17 @@
         <v>21</v>
       </c>
       <c r="D18" s="21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="22">
         <v>3</v>
       </c>
       <c r="F18" s="23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G18" s="24">
         <f>SUM(D18:F18)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2311,17 +2282,17 @@
         <v>22</v>
       </c>
       <c r="D19" s="21">
+        <v>4</v>
+      </c>
+      <c r="E19" s="22">
         <v>5</v>
       </c>
-      <c r="E19" s="22">
+      <c r="F19" s="23">
         <v>3</v>
-      </c>
-      <c r="F19" s="23">
-        <v>2</v>
       </c>
       <c r="G19" s="24">
         <f>SUM(D19:F19)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2339,17 +2310,17 @@
         <v>23</v>
       </c>
       <c r="D20" s="21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" s="23">
         <v>4</v>
       </c>
       <c r="G20" s="24">
         <f>SUM(D20:F20)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2370,14 +2341,14 @@
         <v>4</v>
       </c>
       <c r="E21" s="22">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F21" s="23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G21" s="24">
         <f>SUM(D21:F21)</f>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2398,14 +2369,14 @@
         <v>4</v>
       </c>
       <c r="E22" s="22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F22" s="23">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G22" s="24">
         <f>SUM(D22:F22)</f>
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2423,17 +2394,17 @@
         <v>26</v>
       </c>
       <c r="D23" s="21">
+        <v>3</v>
+      </c>
+      <c r="E23" s="22">
+        <v>10</v>
+      </c>
+      <c r="F23" s="23">
         <v>4</v>
-      </c>
-      <c r="E23" s="22">
-        <v>2</v>
-      </c>
-      <c r="F23" s="23">
-        <v>7</v>
       </c>
       <c r="G23" s="24">
         <f>SUM(D23:F23)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2485,11 +2456,11 @@
         <v>2</v>
       </c>
       <c r="F25" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G25" s="24">
         <f>SUM(D25:F25)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2510,10 +2481,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G26" s="24">
         <f>SUM(D26:F26)</f>
@@ -2541,11 +2512,11 @@
         <v>1</v>
       </c>
       <c r="F27" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G27" s="24">
         <f>SUM(D27:F27)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2567,19 +2538,19 @@
       </c>
       <c r="D28" s="32">
         <f>SUM(D3:D27)</f>
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="E28" s="32">
         <f>SUM(E3:E27)</f>
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="F28" s="32">
         <f>SUM(F3:F27)</f>
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G28" s="33">
         <f>SUM(G3:G27)</f>
-        <v>725</v>
+        <v>736</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>

</xml_diff>